<commit_message>
graph dfs bfs check circle
</commit_message>
<xml_diff>
--- a/leetcode/leetcodebk.xlsx
+++ b/leetcode/leetcodebk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workshop\git\Algorithm\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1296897-2E54-4C3D-AA81-CDC684938F5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4B62F8-2441-43BB-881B-A373CB525B61}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="problem" sheetId="1" r:id="rId1"/>
@@ -5901,7 +5901,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2657476" y="4019550"/>
+          <a:off x="2657476" y="9220200"/>
           <a:ext cx="371474" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -7318,8 +7318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:I33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7766,8 +7766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33018385-90F7-499C-8B43-4C2BDB7FF198}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E102" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -8408,7 +8408,8 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D6134F69-DF9E-498D-B47C-51B3103DEDC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>